<commit_message>
update template to change software lifecycles to releases
</commit_message>
<xml_diff>
--- a/skill-grading-template.xlsx
+++ b/skill-grading-template.xlsx
@@ -37,6 +37,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>A maxim would be: "test everything that can possibly break."
 	-Ken Taylor</t>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
   <si>
     <t>Career Development</t>
   </si>
@@ -339,13 +340,25 @@
   </si>
   <si>
     <t>MCSD: Web Applications</t>
+  </si>
+  <si>
+    <t># of completed software project major/minor releases</t>
+  </si>
+  <si>
+    <t>Earned</t>
+  </si>
+  <si>
+    <t>Expires</t>
+  </si>
+  <si>
+    <t>License #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -354,40 +367,48 @@
     <font>
       <sz val="24"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF252525"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -399,6 +420,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -430,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -466,6 +493,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -960,13 +988,13 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -998,7 +1026,7 @@
       </c>
       <c r="C14" s="5"/>
       <c r="H14" s="7" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1012,7 +1040,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1032,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -1041,7 +1069,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -1054,11 +1082,17 @@
       <c r="H18" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1068,7 +1102,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -1077,7 +1111,7 @@
       </c>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
@@ -1093,7 +1127,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
@@ -1102,7 +1136,7 @@
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -1110,7 +1144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
@@ -1118,7 +1152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1127,7 +1161,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>49</v>
       </c>
@@ -1136,10 +1170,10 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
     </row>
   </sheetData>
@@ -1237,13 +1271,13 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">

</xml_diff>

<commit_message>
added plan notes tab for coaching
</commit_message>
<xml_diff>
--- a/skill-grading-template.xlsx
+++ b/skill-grading-template.xlsx
@@ -14,8 +14,9 @@
   <sheets>
     <sheet name="Doe, John" sheetId="2" r:id="rId1"/>
     <sheet name="Doe, Jane" sheetId="5" r:id="rId2"/>
-    <sheet name="SWE Disciplines" sheetId="9" r:id="rId3"/>
-    <sheet name="Dreyfus Model" sheetId="10" r:id="rId4"/>
+    <sheet name="Plan Notes" sheetId="11" r:id="rId3"/>
+    <sheet name="SWE Disciplines" sheetId="9" r:id="rId4"/>
+    <sheet name="Dreyfus Model" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
   <si>
     <t>Career Development</t>
   </si>
@@ -352,13 +353,19 @@
   </si>
   <si>
     <t>License #</t>
+  </si>
+  <si>
+    <t>Plan Notes</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -429,6 +436,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -457,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -494,10 +507,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -988,13 +1003,13 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -1271,13 +1286,13 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -1480,6 +1495,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="22"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G16"/>
   <sheetViews>
@@ -1667,7 +1715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>

</xml_diff>

<commit_message>
add row color to disciplines assessment
</commit_message>
<xml_diff>
--- a/skill-grading-template.xlsx
+++ b/skill-grading-template.xlsx
@@ -100,9 +100,6 @@
     <t>Business modeling</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t># of completed software project life-cycles</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Analysis and design</t>
   </si>
   <si>
-    <t>Senior Software Engineer</t>
-  </si>
-  <si>
     <t># peers or jr. engineers mentored</t>
   </si>
   <si>
@@ -359,13 +353,19 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Sr Software Engineer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -442,6 +442,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -470,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -508,17 +521,151 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -544,8 +691,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -653,6 +800,36 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A13:F27" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A13:F27"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Software Engineering Discipline" dataDxfId="6"/>
+    <tableColumn id="2" name="Novice" dataDxfId="5"/>
+    <tableColumn id="3" name="Advanced Beginner" dataDxfId="4"/>
+    <tableColumn id="4" name="Competent"/>
+    <tableColumn id="5" name="Proficient"/>
+    <tableColumn id="6" name="Expert"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:F28" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A13:F28"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Software Engineering Discipline" dataDxfId="2"/>
+    <tableColumn id="2" name="Novice"/>
+    <tableColumn id="3" name="Advanced Beginner" dataDxfId="1"/>
+    <tableColumn id="4" name="Competent"/>
+    <tableColumn id="5" name="Proficient"/>
+    <tableColumn id="6" name="Expert"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -921,7 +1098,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -930,6 +1107,8 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
     <col min="8" max="8" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -943,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -959,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1003,31 +1182,31 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="6"/>
@@ -1037,11 +1216,11 @@
         <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="C14" s="5"/>
       <c r="H14" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1049,13 +1228,13 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1063,13 +1242,13 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="I16" s="5">
         <v>0</v>
@@ -1077,111 +1256,111 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="E18" s="5"/>
       <c r="H18" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I18" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" s="18" t="s">
         <v>98</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -1196,6 +1375,10 @@
     <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1204,15 +1387,17 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
     <col min="8" max="8" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1225,15 +1410,15 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>94</v>
+      <c r="B3" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="28">
         <v>42261</v>
       </c>
     </row>
@@ -1241,8 +1426,8 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
+      <c r="B5" s="29" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1286,31 +1471,31 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="6"/>
@@ -1323,10 +1508,10 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="I14" s="5">
         <v>15</v>
@@ -1334,15 +1519,15 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I15" s="5">
         <v>5</v>
@@ -1350,16 +1535,16 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I16" s="5">
         <v>5</v>
@@ -1367,40 +1552,40 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="E18" s="5"/>
       <c r="H18" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I19" s="20">
         <v>41913</v>
@@ -1408,76 +1593,76 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5"/>
       <c r="D22" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5"/>
       <c r="D25" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1491,6 +1676,9 @@
     <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1505,8 +1693,8 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>101</v>
+      <c r="A1" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -1516,10 +1704,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1543,13 +1731,13 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1557,144 +1745,144 @@
         <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1732,12 +1920,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1745,13 +1933,13 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1762,20 +1950,20 @@
         <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="C6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1791,25 +1979,25 @@
         <v>11</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="C10" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="C11" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="C12" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1824,37 +2012,37 @@
         <v>12</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="C15" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="C16" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="C17" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="C18" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="C19" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,37 +2057,37 @@
         <v>13</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="C22" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="C23" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="C24" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="C25" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="C26" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1915,37 +2103,37 @@
         <v>14</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="C29" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="C30" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="C31" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="C32" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="C33" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>